<commit_message>
adding final preso pdf
</commit_message>
<xml_diff>
--- a/analysis/elasticity.xlsx
+++ b/analysis/elasticity.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pwilliams/Projects/regression-mei-team-proj/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18DEB798-3A45-9646-967B-881FF8DC8037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7AED63FA-010D-3C4F-B617-2992855395CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15780"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gdp" sheetId="1" r:id="rId1"/>
+    <sheet name="alc" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>fm_labor</t>
   </si>
@@ -496,8 +498,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -540,52 +543,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -899,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
@@ -3056,4 +3062,1603 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54:J54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B3">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5.4419496473789</v>
+      </c>
+      <c r="E3">
+        <v>8.2757137082810406</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>6.7700395145309402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B4">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>5.6185336430453896</v>
+      </c>
+      <c r="E4">
+        <v>8.4168944166749906</v>
+      </c>
+      <c r="F4">
+        <v>0.31020408163265301</v>
+      </c>
+      <c r="G4">
+        <v>6.9331525136286301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B5">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>5.7977598278122899</v>
+      </c>
+      <c r="E5">
+        <v>8.5604602937552094</v>
+      </c>
+      <c r="F5">
+        <v>0.62040816326530601</v>
+      </c>
+      <c r="G5">
+        <v>7.0986010313180996</v>
+      </c>
+      <c r="I5" s="1">
+        <f>F5/F4-1</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>G5/G4-1</f>
+        <v>2.3863389326030937E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B6">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5.9795429057692902</v>
+      </c>
+      <c r="E6">
+        <v>8.7065257304877797</v>
+      </c>
+      <c r="F6">
+        <v>0.93061224489795902</v>
+      </c>
+      <c r="G6">
+        <v>7.2663961094587499</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I52" si="0">F6/F5-1</f>
+        <v>0.5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J52" si="1">G6/G5-1</f>
+        <v>2.3637767131912346E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B7">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6.1637866904690499</v>
+      </c>
+      <c r="E7">
+        <v>8.8552158310900992</v>
+      </c>
+      <c r="F7">
+        <v>1.24081632653061</v>
+      </c>
+      <c r="G7">
+        <v>7.4365487381939204</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333126</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>2.3416371220622123E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B8">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>6.3503833054771501</v>
+      </c>
+      <c r="E8">
+        <v>9.0066672157929393</v>
+      </c>
+      <c r="F8">
+        <v>1.5510204081632699</v>
+      </c>
+      <c r="G8">
+        <v>7.60906985667095</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.250000000000006</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>2.3199083950188548E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B9">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>6.5392124351977703</v>
+      </c>
+      <c r="E9">
+        <v>9.1610287732231708</v>
+      </c>
+      <c r="F9">
+        <v>1.86122448979592</v>
+      </c>
+      <c r="G9">
+        <v>7.7839703537444498</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999751</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>2.298579200454598E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B10">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>6.7301406722901698</v>
+      </c>
+      <c r="E10">
+        <v>9.3184623160965199</v>
+      </c>
+      <c r="F10">
+        <v>2.1714285714285699</v>
+      </c>
+      <c r="G10">
+        <v>7.96126106866366</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666474</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>2.277638619652822E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B11">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>6.9230210206801601</v>
+      </c>
+      <c r="E11">
+        <v>9.4791430812206201</v>
+      </c>
+      <c r="F11">
+        <v>2.4816326530612201</v>
+      </c>
+      <c r="G11">
+        <v>8.14095279174437</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714168</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>2.2570761281525575E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B12">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>7.1176926265877603</v>
+      </c>
+      <c r="E12">
+        <v>9.6432600013910594</v>
+      </c>
+      <c r="F12">
+        <v>2.7918367346938799</v>
+      </c>
+      <c r="G12">
+        <v>8.3230562650256701</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.12500000000000289</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>2.2368815781117046E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B13">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>7.3139808228509597</v>
+      </c>
+      <c r="E13">
+        <v>9.81101566390433</v>
+      </c>
+      <c r="F13">
+        <v>3.1020408163265301</v>
+      </c>
+      <c r="G13">
+        <v>8.5075821829122091</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11111111111111005</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>2.217045181611188E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B14">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>7.5116975821127596</v>
+      </c>
+      <c r="E14">
+        <v>9.9826258601241999</v>
+      </c>
+      <c r="F14">
+        <v>3.4122448979591802</v>
+      </c>
+      <c r="G14">
+        <v>8.6945411928023297</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9999999999998979E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>2.1975574948383647E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B15">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>7.7106424793445996</v>
+      </c>
+      <c r="E15">
+        <v>10.158318625631701</v>
+      </c>
+      <c r="F15">
+        <v>3.7224489795918401</v>
+      </c>
+      <c r="G15">
+        <v>8.8839438957025507</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0909090909093049E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>2.1784094030978363E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B16">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>7.9106042601829403</v>
+      </c>
+      <c r="E16">
+        <v>10.3383326744851</v>
+      </c>
+      <c r="F16">
+        <v>4.0326530612244902</v>
+      </c>
+      <c r="G16">
+        <v>9.0758008468286597</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3333333333332371E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>2.1595921065971302E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B17">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>8.1113630947872508</v>
+      </c>
+      <c r="E17">
+        <v>10.522915147885501</v>
+      </c>
+      <c r="F17">
+        <v>4.3428571428571399</v>
+      </c>
+      <c r="G17">
+        <v>9.2701225561941207</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>7.6923076923075984E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>2.1410971069661944E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B18">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>8.3126935639063895</v>
+      </c>
+      <c r="E18">
+        <v>10.7123186305622</v>
+      </c>
+      <c r="F18">
+        <v>4.6530612244898002</v>
+      </c>
+      <c r="G18">
+        <v>9.4669194891858108</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>7.1428571428573173E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>2.1229161944595232E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B19">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>8.5143683726033608</v>
+      </c>
+      <c r="E19">
+        <v>10.9067974394328</v>
+      </c>
+      <c r="F19">
+        <v>4.9632653061224499</v>
+      </c>
+      <c r="G19">
+        <v>9.6662020671277595</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6666666666665986E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>2.1050414358080527E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B20">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>8.7161627185911392</v>
+      </c>
+      <c r="E20">
+        <v>11.106603257586601</v>
+      </c>
+      <c r="F20">
+        <v>5.2734693877551004</v>
+      </c>
+      <c r="G20">
+        <v>9.8679806678330309</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2499999999999556E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>2.087465162677149E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B21">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>8.9178591615449996</v>
+      </c>
+      <c r="E21">
+        <v>11.311980267228099</v>
+      </c>
+      <c r="F21">
+        <v>5.5836734693877599</v>
+      </c>
+      <c r="G21">
+        <v>10.072265626144199</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8823529411765829E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>2.0701799606993809E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B22">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>9.1192527570846895</v>
+      </c>
+      <c r="E22">
+        <v>11.523160017891099</v>
+      </c>
+      <c r="F22">
+        <v>5.8938775510204104</v>
+      </c>
+      <c r="G22">
+        <v>10.279067234463</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555136E-2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>2.0531786590497925E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B23">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>9.3201561484847701</v>
+      </c>
+      <c r="E23">
+        <v>11.7403563368657</v>
+      </c>
+      <c r="F23">
+        <v>6.2040816326530601</v>
+      </c>
+      <c r="G23">
+        <v>10.4883957432684</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>5.2631578947367919E-2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>2.0364543205202201E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B24">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>9.5204042663660093</v>
+      </c>
+      <c r="E24">
+        <v>11.963760631589</v>
+      </c>
+      <c r="F24">
+        <v>6.5142857142857098</v>
+      </c>
+      <c r="G24">
+        <v>10.7002613616252</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999378E-2</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>2.0200002320924781E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B25">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>9.7198582851354907</v>
+      </c>
+      <c r="E25">
+        <v>12.1935379352325</v>
+      </c>
+      <c r="F25">
+        <v>6.8244897959183701</v>
+      </c>
+      <c r="G25">
+        <v>10.914674257682099</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="0"/>
+        <v>4.7619047619048782E-2</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>2.0038098959513029E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B26">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>9.9184085315536201</v>
+      </c>
+      <c r="E26">
+        <v>12.429824000110299</v>
+      </c>
+      <c r="F26">
+        <v>7.1346938775510198</v>
+      </c>
+      <c r="G26">
+        <v>11.1316445591592</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="0"/>
+        <v>4.545454545454497E-2</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>1.9878770209233787E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B27">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>10.1159761323396</v>
+      </c>
+      <c r="E27">
+        <v>12.672723651999799</v>
+      </c>
+      <c r="F27">
+        <v>7.4448979591836704</v>
+      </c>
+      <c r="G27">
+        <v>11.3511823538268</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3478260869564966E-2</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>1.9721955143363168E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B28">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>10.312513310619799</v>
+      </c>
+      <c r="E28">
+        <v>12.9223104955702</v>
+      </c>
+      <c r="F28">
+        <v>7.7551020408163298</v>
+      </c>
+      <c r="G28">
+        <v>11.573297689974501</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1666666666667629E-2</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>1.9567594742482486E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B29">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>10.508002374255</v>
+      </c>
+      <c r="E29">
+        <v>13.178627927885501</v>
+      </c>
+      <c r="F29">
+        <v>8.0653061224489804</v>
+      </c>
+      <c r="G29">
+        <v>11.7980005768711</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9999999999999591E-2</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>1.9415631820414614E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B30">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>10.7024535596672</v>
+      </c>
+      <c r="E30">
+        <v>13.4416912963637</v>
+      </c>
+      <c r="F30">
+        <v>8.3755102040816301</v>
+      </c>
+      <c r="G30">
+        <v>12.025300985215599</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8461538461538103E-2</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>1.9266010953593371E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B31">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>10.8959019838054</v>
+      </c>
+      <c r="E31">
+        <v>13.7114909485522</v>
+      </c>
+      <c r="F31">
+        <v>8.6857142857142904</v>
+      </c>
+      <c r="G31">
+        <v>12.2552088475797</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7037037037037868E-2</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>1.9118678413684531E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B32">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>11.0884040038818</v>
+      </c>
+      <c r="E32">
+        <v>13.987995874091901</v>
+      </c>
+      <c r="F32">
+        <v>8.9959183673469401</v>
+      </c>
+      <c r="G32">
+        <v>12.487734058841999</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5714285714285365E-2</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>1.8973582103271935E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B33">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>11.2800332888008</v>
+      </c>
+      <c r="E33">
+        <v>14.2711576349475</v>
+      </c>
+      <c r="F33">
+        <v>9.3061224489795897</v>
+      </c>
+      <c r="G33">
+        <v>12.7228864766137</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.448275862068928E-2</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>1.8830671494417306E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B34">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>11.470876875288999</v>
+      </c>
+      <c r="E34">
+        <v>14.5609143108976</v>
+      </c>
+      <c r="F34">
+        <v>9.6163265306122394</v>
+      </c>
+      <c r="G34">
+        <v>12.960675921656801</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333332993E-2</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>1.8689897570035585E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B35">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>11.661031427790601</v>
+      </c>
+      <c r="E35">
+        <v>14.8571942412211</v>
+      </c>
+      <c r="F35">
+        <v>9.9265306122448997</v>
+      </c>
+      <c r="G35">
+        <v>13.201112178294</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2258064516129892E-2</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>1.8551212767803138E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B36">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>11.8505998572429</v>
+      </c>
+      <c r="E36">
+        <v>15.1599194074675</v>
+      </c>
+      <c r="F36">
+        <v>10.236734693877599</v>
+      </c>
+      <c r="G36">
+        <v>13.444204994811599</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1250000000004663E-2</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>1.8414570926630347E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B37">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>12.0396883909129</v>
+      </c>
+      <c r="E37">
+        <v>15.469008365129699</v>
+      </c>
+      <c r="F37">
+        <v>10.546938775510201</v>
+      </c>
+      <c r="G37">
+        <v>13.6899640838545</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0303030303025169E-2</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>1.8279927235395732E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B38">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>12.228404131037101</v>
+      </c>
+      <c r="E38">
+        <v>15.7843786864804</v>
+      </c>
+      <c r="F38">
+        <v>10.8571428571429</v>
+      </c>
+      <c r="G38">
+        <v>13.938399122814699</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9411764705886689E-2</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>1.8147238184006209E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B39">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>12.4168530978421</v>
+      </c>
+      <c r="E39">
+        <v>16.105948918993199</v>
+      </c>
+      <c r="F39">
+        <v>11.1673469387755</v>
+      </c>
+      <c r="G39">
+        <v>14.189519754211901</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8571428571423585E-2</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>1.8016461516456417E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B40">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>12.605138723386601</v>
+      </c>
+      <c r="E40">
+        <v>16.4336400929107</v>
+      </c>
+      <c r="F40">
+        <v>11.4775510204082</v>
+      </c>
+      <c r="G40">
+        <v>14.4433355860681</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7777777777781898E-2</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>1.7887556186026554E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B41">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>12.7933607452754</v>
+      </c>
+      <c r="E41">
+        <v>16.767376828909399</v>
+      </c>
+      <c r="F41">
+        <v>11.7877551020408</v>
+      </c>
+      <c r="G41">
+        <v>14.699856192275201</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="0"/>
+        <v>2.702702702702231E-2</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>1.7760482312308756E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B42">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>12.9816144413582</v>
+      </c>
+      <c r="E42">
+        <v>17.107088104749799</v>
+      </c>
+      <c r="F42">
+        <v>12.097959183673501</v>
+      </c>
+      <c r="G42">
+        <v>14.9590911129562</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6315789473688289E-2</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>1.7635201140078438E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B43">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>13.1699901454621</v>
+      </c>
+      <c r="E43">
+        <v>17.452707740862401</v>
+      </c>
+      <c r="F43">
+        <v>12.408163265306101</v>
+      </c>
+      <c r="G43">
+        <v>15.2210498548198</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5641025641021109E-2</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>1.7511674999874494E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B44">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>13.358572987654499</v>
+      </c>
+      <c r="E44">
+        <v>17.8041746613765</v>
+      </c>
+      <c r="F44">
+        <v>12.7183673469388</v>
+      </c>
+      <c r="G44">
+        <v>15.485741891509299</v>
+      </c>
+      <c r="I44" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5000000000003686E-2</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>1.7389867270271475E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B45">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>13.5474428085464</v>
+      </c>
+      <c r="E45">
+        <v>18.161432981078999</v>
+      </c>
+      <c r="F45">
+        <v>13.0285714285714</v>
+      </c>
+      <c r="G45">
+        <v>15.7531766639453</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4390243902434827E-2</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>1.726974234167189E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B46">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>13.7366742043131</v>
+      </c>
+      <c r="E46">
+        <v>18.524431961631699</v>
+      </c>
+      <c r="F46">
+        <v>13.338775510204099</v>
+      </c>
+      <c r="G46">
+        <v>16.023363580662199</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" si="0"/>
+        <v>2.38095238095275E-2</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>1.7151265581581532E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B47">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>13.9263366664293</v>
+      </c>
+      <c r="E47">
+        <v>18.893125873045399</v>
+      </c>
+      <c r="F47">
+        <v>13.648979591836699</v>
+      </c>
+      <c r="G47">
+        <v>16.296312018139201</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3255813953484417E-2</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>1.7034403301339873E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B48">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>14.116494787017</v>
+      </c>
+      <c r="E48">
+        <v>19.267473789517801</v>
+      </c>
+      <c r="F48">
+        <v>13.959183673469401</v>
+      </c>
+      <c r="G48">
+        <v>16.5720313211262</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="0"/>
+        <v>2.272727272727626E-2</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>1.6919122724215141E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B49">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>14.3072085068411</v>
+      </c>
+      <c r="E49">
+        <v>19.647439342599402</v>
+      </c>
+      <c r="F49">
+        <v>14.269387755102001</v>
+      </c>
+      <c r="G49">
+        <v>16.8505308029631</v>
+      </c>
+      <c r="I49" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2222222222218369E-2</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>1.6805391954688442E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B50">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>14.4985333882451</v>
+      </c>
+      <c r="E50">
+        <v>20.032990449394099</v>
+      </c>
+      <c r="F50">
+        <v>14.5795918367347</v>
+      </c>
+      <c r="G50">
+        <v>17.131819745895001</v>
+      </c>
+      <c r="I50" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1739130434785814E-2</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>1.6693179949111014E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B51">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>14.690520899686099</v>
+      </c>
+      <c r="E51">
+        <v>20.424099029138599</v>
+      </c>
+      <c r="F51">
+        <v>14.8897959183673</v>
+      </c>
+      <c r="G51">
+        <v>17.415907401381201</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1276595744677218E-2</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>1.6582456487395092E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>0.71365432098765402</v>
+      </c>
+      <c r="B52">
+        <v>9.5131559242322705</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>14.8832187020652</v>
+      </c>
+      <c r="E52">
+        <v>20.820740717963801</v>
+      </c>
+      <c r="F52">
+        <v>15.2</v>
+      </c>
+      <c r="G52">
+        <v>17.7028029903997</v>
+      </c>
+      <c r="I52" s="1">
+        <f t="shared" si="0"/>
+        <v>2.083333333333659E-2</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="1"/>
+        <v>1.6473192145919802E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I54" s="2">
+        <f>AVERAGE(I16:I52)</f>
+        <v>3.888972514018306E-2</v>
+      </c>
+      <c r="J54" s="2">
+        <f>AVERAGE(J16:J52)</f>
+        <v>1.8810353789823875E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>